<commit_message>
Added matlab commands for clipboard
</commit_message>
<xml_diff>
--- a/Regression annual, 1991-2010 (EIA data).xlsx
+++ b/Regression annual, 1991-2010 (EIA data).xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\home.ansatt.ntnu.no\valeriyk\System\Skrivebord\GitHub\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\home.ansatt.ntnu.no\valeriyk\system\Skrivebord\GitHub\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>TotRetPrem</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>Value weighted of E&amp;P and Int Indexes</t>
+  </si>
+  <si>
+    <t>EPRetPrem</t>
+  </si>
+  <si>
+    <t>IntRetPrem</t>
   </si>
 </sst>
 </file>
@@ -380,15 +386,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection sqref="A1:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -396,25 +402,31 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1991</v>
       </c>
@@ -422,25 +434,31 @@
         <v>-0.20136443935385712</v>
       </c>
       <c r="C2">
+        <v>-0.40672404853143224</v>
+      </c>
+      <c r="D2">
+        <v>-1990.9054517596526</v>
+      </c>
+      <c r="E2">
         <v>0.20926703027355376</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>2.0966855027074295E-3</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>-3.5842995686358313E-2</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>-7.9177971122961294E-2</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>0</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1992</v>
       </c>
@@ -448,19 +466,25 @@
         <v>-9.5192346979379797E-2</v>
       </c>
       <c r="C3">
+        <v>-0.12331656348690673</v>
+      </c>
+      <c r="D3">
+        <v>-1992.0237147063688</v>
+      </c>
+      <c r="E3">
         <v>1.0342631514950115E-2</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>-9.060415895212226E-3</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>-2.4334135057781366E-2</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>-0.20048767271742074</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1993</v>
       </c>
@@ -468,19 +492,25 @@
         <v>1.1261214009137946E-2</v>
       </c>
       <c r="C4">
+        <v>-7.2336404528358073E-2</v>
+      </c>
+      <c r="D4">
+        <v>-1992.8621240279881</v>
+      </c>
+      <c r="E4">
         <v>4.055156327594979E-2</v>
       </c>
-      <c r="D4">
+      <c r="F4">
         <v>-1.4030545914636164E-2</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>-2.3832056848301447E-2</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>7.8066757031514736E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1994</v>
       </c>
@@ -488,19 +518,25 @@
         <v>-0.14118449428337404</v>
       </c>
       <c r="C5">
+        <v>-0.28112312216259605</v>
+      </c>
+      <c r="D5">
+        <v>-1993.9851908843464</v>
+      </c>
+      <c r="E5">
         <v>-5.7892909883771229E-2</v>
       </c>
-      <c r="D5">
+      <c r="F5">
         <v>9.4851344531378182E-3</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>-5.2572487065102591E-3</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>-0.12557463360968135</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>1995</v>
       </c>
@@ -508,19 +544,25 @@
         <v>0.15451420882669531</v>
       </c>
       <c r="C6">
+        <v>9.5414760658868059E-2</v>
+      </c>
+      <c r="D6">
+        <v>-1994.7742997199041</v>
+      </c>
+      <c r="E6">
         <v>0.28620655551673757</v>
       </c>
-      <c r="D6">
+      <c r="F6">
         <v>-1.2429128943433326E-2</v>
       </c>
-      <c r="E6">
+      <c r="G6">
         <v>2.2540098265448733E-3</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <v>-2.9431588407099529E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>1996</v>
       </c>
@@ -528,19 +570,25 @@
         <v>0.20556859420558091</v>
       </c>
       <c r="C7">
+        <v>0.22092369660558633</v>
+      </c>
+      <c r="D7">
+        <v>-1995.8183037051381</v>
+      </c>
+      <c r="E7">
         <v>0.15253666068945609</v>
       </c>
-      <c r="D7">
+      <c r="F7">
         <v>4.0228114705200668E-3</v>
       </c>
-      <c r="E7">
+      <c r="G7">
         <v>-2.2589656877813409E-3</v>
       </c>
-      <c r="F7">
+      <c r="H7">
         <v>0.10583333333333333</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1997</v>
       </c>
@@ -548,19 +596,25 @@
         <v>2.2531862991482181E-2</v>
       </c>
       <c r="C8">
+        <v>-0.14768340458183332</v>
+      </c>
+      <c r="D8">
+        <v>-1996.8175564642638</v>
+      </c>
+      <c r="E8">
         <v>0.25948181831792277</v>
       </c>
-      <c r="D8">
+      <c r="F8">
         <v>-3.9002194255675075E-4</v>
       </c>
-      <c r="E8">
+      <c r="G8">
         <v>1.3139033277959282E-2</v>
       </c>
-      <c r="F8">
+      <c r="H8">
         <v>0.15490245331993635</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>1998</v>
       </c>
@@ -568,19 +622,25 @@
         <v>-0.11556120642452433</v>
       </c>
       <c r="C9">
+        <v>-0.44408825558245291</v>
+      </c>
+      <c r="D9">
+        <v>-1997.9429986830105</v>
+      </c>
+      <c r="E9">
         <v>0.21888589065342307</v>
       </c>
-      <c r="D9">
+      <c r="F9">
         <v>-1.0066662883766097E-2</v>
       </c>
-      <c r="E9">
+      <c r="G9">
         <v>-4.0509224823883618E-2</v>
       </c>
-      <c r="F9">
+      <c r="H9">
         <v>-0.16947002102515768</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>1999</v>
       </c>
@@ -588,19 +648,25 @@
         <v>0.10963582408296163</v>
       </c>
       <c r="C10">
+        <v>0.11300284903673877</v>
+      </c>
+      <c r="D10">
+        <v>-1998.8622551868068</v>
+      </c>
+      <c r="E10">
         <v>0.14886046704458014</v>
       </c>
-      <c r="D10">
+      <c r="F10">
         <v>-2.8753037408824355E-2</v>
       </c>
-      <c r="E10">
+      <c r="G10">
         <v>2.6705025065031165E-2</v>
       </c>
-      <c r="F10">
+      <c r="H10">
         <v>-0.17336650517218805</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>2000</v>
       </c>
@@ -608,19 +674,25 @@
         <v>0.22639794259110921</v>
       </c>
       <c r="C11">
+        <v>0.39226784987588126</v>
+      </c>
+      <c r="D11">
+        <v>-1999.9244003603874</v>
+      </c>
+      <c r="E11">
         <v>-0.15959184686064318</v>
       </c>
-      <c r="D11">
+      <c r="F11">
         <v>9.0717706218465498E-3</v>
       </c>
-      <c r="E11">
+      <c r="G11">
         <v>3.9265627726546765E-2</v>
       </c>
-      <c r="F11">
+      <c r="H11">
         <v>0.54638576482390833</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>2001</v>
       </c>
@@ -628,19 +700,25 @@
         <v>-0.16672122682288931</v>
       </c>
       <c r="C12">
+        <v>-0.28086053266448835</v>
+      </c>
+      <c r="D12">
+        <v>-2001.0832951564967</v>
+      </c>
+      <c r="E12">
         <v>-0.16432693157331701</v>
       </c>
-      <c r="D12">
+      <c r="F12">
         <v>8.902134462046218E-3</v>
       </c>
-      <c r="E12">
+      <c r="G12">
         <v>2.7249214554871372E-2</v>
       </c>
-      <c r="F12">
+      <c r="H12">
         <v>0.214122306825554</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>2002</v>
       </c>
@@ -648,19 +726,25 @@
         <v>-0.11344253187320717</v>
       </c>
       <c r="C13">
+        <v>-4.3590047731240672E-2</v>
+      </c>
+      <c r="D13">
+        <v>-2002.1586287406246</v>
+      </c>
+      <c r="E13">
         <v>-0.24965963981693273</v>
       </c>
-      <c r="D13">
+      <c r="F13">
         <v>-2.4373980495658636E-2</v>
       </c>
-      <c r="E13">
+      <c r="G13">
         <v>1.5314205245555358E-2</v>
       </c>
-      <c r="F13">
+      <c r="H13">
         <v>-0.21618201248664154</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>2003</v>
       </c>
@@ -668,19 +752,25 @@
         <v>0.21529016858624037</v>
       </c>
       <c r="C14">
+        <v>0.18959209869171162</v>
+      </c>
+      <c r="D14">
+        <v>-2002.7942619943894</v>
+      </c>
+      <c r="E14">
         <v>0.253703999856075</v>
       </c>
-      <c r="D14">
+      <c r="F14">
         <v>-3.6340833138966029E-3</v>
       </c>
-      <c r="E14">
+      <c r="G14">
         <v>-8.1050624133150208E-3</v>
       </c>
-      <c r="F14">
+      <c r="H14">
         <v>0.17803451616375443</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>2004</v>
       </c>
@@ -688,19 +778,25 @@
         <v>0.27524076425712213</v>
       </c>
       <c r="C15">
+        <v>0.27435964466695179</v>
+      </c>
+      <c r="D15">
+        <v>-2003.7723046200983</v>
+      </c>
+      <c r="E15">
         <v>7.6234524105044374E-2</v>
       </c>
-      <c r="D15">
+      <c r="F15">
         <v>-2.7220244151345878E-2</v>
       </c>
-      <c r="E15">
+      <c r="G15">
         <v>1.089297418770964E-3</v>
       </c>
-      <c r="F15">
+      <c r="H15">
         <v>0.12865105229494717</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>2005</v>
       </c>
@@ -708,19 +804,25 @@
         <v>0.37777709139066373</v>
       </c>
       <c r="C16">
+        <v>0.47076701936886745</v>
+      </c>
+      <c r="D16">
+        <v>-2004.859592737125</v>
+      </c>
+      <c r="E16">
         <v>-1.4897735167749906E-3</v>
       </c>
-      <c r="D16">
+      <c r="F16">
         <v>-3.7697688494401083E-2</v>
       </c>
-      <c r="E16">
+      <c r="G16">
         <v>4.4235344002444311E-2</v>
       </c>
-      <c r="F16">
+      <c r="H16">
         <v>0.18795369295949482</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>2006</v>
       </c>
@@ -728,19 +830,25 @@
         <v>0.14460216011094199</v>
       </c>
       <c r="C17">
+        <v>-8.2649175991275983E-3</v>
+      </c>
+      <c r="D17">
+        <v>-2005.72286975985</v>
+      </c>
+      <c r="E17">
         <v>8.8894317577182858E-2</v>
       </c>
-      <c r="D17">
+      <c r="F17">
         <v>8.9051513614827812E-3</v>
       </c>
-      <c r="E17">
+      <c r="G17">
         <v>5.9415932427067065E-3</v>
       </c>
-      <c r="F17">
+      <c r="H17">
         <v>0.1682567807005588</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>2007</v>
       </c>
@@ -748,19 +856,25 @@
         <v>0.30788445915514884</v>
       </c>
       <c r="C18">
+        <v>0.31700140929592346</v>
+      </c>
+      <c r="D18">
+        <v>-2006.7583219905407</v>
+      </c>
+      <c r="E18">
         <v>-8.2042697098573467E-3</v>
       </c>
-      <c r="D18">
+      <c r="F18">
         <v>2.5090386656850844E-2</v>
       </c>
-      <c r="E18">
+      <c r="G18">
         <v>8.5216833819605375E-2</v>
       </c>
-      <c r="F18">
+      <c r="H18">
         <v>-6.9610531023352584E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>2008</v>
       </c>
@@ -768,19 +882,25 @@
         <v>-0.29979059584344714</v>
       </c>
       <c r="C19">
+        <v>-0.44453300322935135</v>
+      </c>
+      <c r="D19">
+        <v>-2008.2676692398031</v>
+      </c>
+      <c r="E19">
         <v>-0.39855793046178661</v>
       </c>
-      <c r="D19">
+      <c r="F19">
         <v>2.4867475859792831E-2</v>
       </c>
-      <c r="E19">
+      <c r="G19">
         <v>-1.7082936755390726E-2</v>
       </c>
-      <c r="F19">
+      <c r="H19">
         <v>6.3264866558320768E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>2009</v>
       </c>
@@ -788,19 +908,25 @@
         <v>0.20114830555434152</v>
       </c>
       <c r="C20">
+        <v>0.34122422383758588</v>
+      </c>
+      <c r="D20">
+        <v>-2009.0405573324622</v>
+      </c>
+      <c r="E20">
         <v>0.23304190534182118</v>
       </c>
-      <c r="D20">
+      <c r="F20">
         <v>3.9845800606202748E-2</v>
       </c>
-      <c r="E20">
+      <c r="G20">
         <v>0.10356389579889906</v>
       </c>
-      <c r="F20">
+      <c r="H20">
         <v>-0.39591543589554712</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>2010</v>
       </c>
@@ -808,19 +934,25 @@
         <v>0.11655117777071604</v>
       </c>
       <c r="C21">
+        <v>8.0503962773586249E-2</v>
+      </c>
+      <c r="D21">
+        <v>-2009.8567614417334</v>
+      </c>
+      <c r="E21">
         <v>0.12642713843408779</v>
       </c>
-      <c r="D21">
+      <c r="F21">
         <v>2.9958456113317867E-2</v>
       </c>
-      <c r="E21">
+      <c r="G21">
         <v>0.12008542590664199</v>
       </c>
-      <c r="F21">
+      <c r="H21">
         <v>0.11608694326738409</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>2011</v>
       </c>
@@ -828,16 +960,22 @@
         <v>2.7518210371873589E-2</v>
       </c>
       <c r="C22">
+        <v>-7.318155143480494E-2</v>
+      </c>
+      <c r="D22">
+        <v>-2010.8882282663687</v>
+      </c>
+      <c r="E22">
         <v>-5.3183661423175915E-4</v>
       </c>
-      <c r="D22">
+      <c r="F22">
         <v>5.866928816659097E-2</v>
       </c>
-      <c r="E22">
+      <c r="G22">
         <v>0.11053808075600986</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>2012</v>
       </c>
@@ -845,16 +983,22 @@
         <v>6.3520335713193451E-3</v>
       </c>
       <c r="C23">
+        <v>1.9752696199697113E-2</v>
+      </c>
+      <c r="D23">
+        <v>-2012.005618743879</v>
+      </c>
+      <c r="E23">
         <v>0.13315690856978843</v>
       </c>
-      <c r="D23">
+      <c r="F23">
         <v>8.593885855197872E-2</v>
       </c>
-      <c r="E23">
+      <c r="G23">
         <v>-4.2993446590625763E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>2013</v>
       </c>
@@ -862,16 +1006,22 @@
         <v>0.21833323259785181</v>
       </c>
       <c r="C24">
+        <v>0.22761349649177387</v>
+      </c>
+      <c r="D24">
+        <v>-2012.8333337165604</v>
+      </c>
+      <c r="E24">
         <v>0.29541249585590784</v>
       </c>
-      <c r="D24">
+      <c r="F24">
         <v>5.9123747537461531E-2</v>
       </c>
-      <c r="E24">
+      <c r="G24">
         <v>9.6252112131267678E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>2014</v>
       </c>
@@ -879,12 +1029,18 @@
         <v>-0.10717203083452383</v>
       </c>
       <c r="C25">
+        <v>-0.1272678823388888</v>
+      </c>
+      <c r="D25">
+        <v>-2014.099589207101</v>
+      </c>
+      <c r="E25">
         <v>0.11360633789337311</v>
       </c>
-      <c r="D25">
+      <c r="F25">
         <v>0.10878235615462215</v>
       </c>
-      <c r="E25">
+      <c r="G25">
         <v>9.0111236977473821E-2</v>
       </c>
     </row>

</xml_diff>